<commit_message>
search two properties and excel data
</commit_message>
<xml_diff>
--- a/TestForgeApp/wwwroot/Uploads/ZgLines.xlsx
+++ b/TestForgeApp/wwwroot/Uploads/ZgLines.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/648fd8a9abc052d2/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Posao\TestForgeApp\TestForgeApp\TestForgeApp\wwwroot\Uploads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A468684A-CF61-4796-A713-F0E0D1A71CC4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{941C698A-FBF7-451D-94DC-69BC28BA2F7D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{670C2877-137E-4727-AAE6-DA3B010F9A8A}"/>
   </bookViews>
@@ -400,10 +400,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0285FEB7-049C-4464-AF09-6F79573A1FE2}">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -476,6 +476,74 @@
         <v>99</v>
       </c>
     </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>30</v>
+      </c>
+      <c r="C5">
+        <v>0.5</v>
+      </c>
+      <c r="D5">
+        <v>20</v>
+      </c>
+      <c r="E5">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>30</v>
+      </c>
+      <c r="C6">
+        <v>0.5</v>
+      </c>
+      <c r="D6">
+        <v>20</v>
+      </c>
+      <c r="E6">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <v>30</v>
+      </c>
+      <c r="C7">
+        <v>0.5</v>
+      </c>
+      <c r="D7">
+        <v>20</v>
+      </c>
+      <c r="E7">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8">
+        <v>30</v>
+      </c>
+      <c r="C8">
+        <v>0.5</v>
+      </c>
+      <c r="D8">
+        <v>20</v>
+      </c>
+      <c r="E8">
+        <v>99</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>